<commit_message>
Lots of changes and commits.
</commit_message>
<xml_diff>
--- a/144F20/Topic 5/Modified Topic 5 DQ 1.xlsx
+++ b/144F20/Topic 5/Modified Topic 5 DQ 1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\Offline\Course Materials\git\Teaching\144F20\Topic 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064CCF57-9EE7-4A7D-856E-B1E0B9167C86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{B7E1C24D-42C2-47C9-BF8E-987C0DCD14F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="19272" windowHeight="11400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <customWorkbookViews>
     <customWorkbookView name="Richard Ketchersid - Personal View" guid="{657628FB-1EAB-42F3-921C-7287B7883E1A}" mergeInterval="0" personalView="1" xWindow="64" yWindow="64" windowWidth="1606" windowHeight="950" tabRatio="500" activeSheetId="1" showComments="commIndAndComment"/>
   </customWorkbookViews>
@@ -618,9 +618,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,30 +627,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -663,26 +642,79 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -692,47 +724,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -760,35 +751,44 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1164,7 +1164,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J1" sqref="J1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,69 +1183,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32" t="s">
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="33"/>
+      <c r="K1" s="41"/>
     </row>
     <row r="2" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18">
+      <c r="A3" s="14">
         <v>15</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <f ca="1">RANDBETWEEN(1,$A$3)</f>
-        <v>5</v>
-      </c>
-      <c r="C3" s="23">
+        <v>8</v>
+      </c>
+      <c r="C3" s="16">
         <f ca="1">RANDBETWEEN(1,$A$3)</f>
-        <v>10</v>
-      </c>
-      <c r="D3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="17">
         <v>1</v>
       </c>
       <c r="F3" s="5">
@@ -1258,21 +1258,21 @@
         <f>ABS(G3-H3)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="24">
+      <c r="B4" s="10"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="17">
         <f>E3+1</f>
         <v>2</v>
       </c>
@@ -1286,19 +1286,19 @@
         <f t="shared" ref="I4:I17" si="1">ABS(G4-H4)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="24">
+      <c r="A5" s="56"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="17">
         <f t="shared" ref="E5:E17" si="2">E4+1</f>
         <v>3</v>
       </c>
@@ -1312,19 +1312,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="24">
+      <c r="A6" s="56"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="17">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -1338,46 +1338,46 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="29" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="24">
+      <c r="A7" s="56"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="17">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="40">
+      <c r="I7" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="47"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="24">
+      <c r="A8" s="57"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="17">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -1387,21 +1387,21 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="40">
+      <c r="I8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="48"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="50"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="24">
+      <c r="A9" s="13"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="17">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -1411,43 +1411,43 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="40">
+      <c r="I9" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J9" s="48"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="50"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C10" s="23"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="24">
+      <c r="C10" s="16"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="17">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="40">
+      <c r="I10" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="50"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="47"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C11" s="23"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="24">
+      <c r="C11" s="16"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="17">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -1457,23 +1457,23 @@
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="40">
+      <c r="I11" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="48"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="24">
+      <c r="C12" s="16"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="17">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -1483,25 +1483,25 @@
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="40">
+      <c r="I12" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="50"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <f ca="1">SUM(F3:F17)</f>
         <v>1</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="24">
+      <c r="B13" s="10"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="17">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -1511,20 +1511,20 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="40">
+      <c r="I13" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="48"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="50"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="47"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="23"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="24">
+      <c r="C14" s="16"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="17">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -1534,23 +1534,23 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="40">
+      <c r="I14" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J14" s="48"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="50"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="47"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="24">
+      <c r="C15" s="16"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="17">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -1560,25 +1560,25 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="40">
+      <c r="I15" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15" s="48"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="50"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="47"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <f ca="1">SUM(F22:F36)</f>
         <v>1</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="24">
+      <c r="B16" s="10"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="17">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
@@ -1588,24 +1588,24 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="40">
+      <c r="I16" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="48"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="47"/>
     </row>
     <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="24">
+      <c r="B17" s="10"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="17">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -1615,85 +1615,85 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="40">
+      <c r="I17" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J17" s="48"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="50"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="11"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="10"/>
+      <c r="D18" s="15"/>
       <c r="H18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="41"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="50"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="47"/>
     </row>
     <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20"/>
-      <c r="B19" s="11"/>
-      <c r="D19" s="22"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="50"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="10"/>
+      <c r="D19" s="15"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="47"/>
     </row>
     <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20"/>
-      <c r="B20" s="11"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="29" t="s">
+      <c r="A20" s="59"/>
+      <c r="B20" s="10"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="50"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="47"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="11"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="28" t="s">
+      <c r="A21" s="59"/>
+      <c r="B21" s="10"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="H21" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="42" t="s">
+      <c r="I21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="48"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="50"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="47"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="10"/>
       <c r="E22" s="5">
         <v>1</v>
       </c>
@@ -1703,42 +1703,42 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="40">
+      <c r="I22" s="25">
         <f>ABS(G22-H22)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="48"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="47"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="10"/>
       <c r="E23" s="5">
         <f>E22+1</f>
         <v>2</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="40">
+      <c r="I23" s="25">
         <f t="shared" ref="I23:I36" si="4">ABS(G23-H23)</f>
         <v>0</v>
       </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="50"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="47"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="59"/>
+      <c r="B24" s="10"/>
       <c r="E24" s="5">
         <f t="shared" ref="E24:E36" si="5">E23+1</f>
         <v>3</v>
@@ -1749,19 +1749,19 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="40">
+      <c r="I24" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J24" s="48"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="50"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="47"/>
     </row>
     <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="21"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="10"/>
       <c r="E25" s="5">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -1772,15 +1772,15 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="40">
+      <c r="I25" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J25" s="48"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="50"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="47"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E26" s="5">
@@ -1793,15 +1793,15 @@
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="40">
+      <c r="I26" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J26" s="48"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="50"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E27" s="5">
@@ -1814,15 +1814,15 @@
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="40">
+      <c r="I27" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J27" s="48"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="50"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="47"/>
     </row>
     <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="5">
@@ -1835,15 +1835,15 @@
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="40">
+      <c r="I28" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J28" s="51"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="53"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
     </row>
     <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E29" s="5">
@@ -1872,17 +1872,17 @@
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
-      <c r="I30" s="40">
+      <c r="I30" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J30" s="63" t="s">
+      <c r="J30" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="K30" s="54"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="56"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="33"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E31" s="5">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="F31" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1899,10 +1899,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K31" s="57"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="59"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="36"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E32" s="5">
@@ -1919,10 +1919,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K32" s="57"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="59"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="36"/>
     </row>
     <row r="33" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E33" s="5">
@@ -1939,10 +1939,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K33" s="60"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="62"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="39"/>
     </row>
     <row r="34" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E34" s="5">
@@ -2010,6 +2010,9 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="10">
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A17:A25"/>
+    <mergeCell ref="D3:D17"/>
     <mergeCell ref="K30:N33"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J7:N28"/>
@@ -2017,9 +2020,6 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="E20:I20"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="D3:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>